<commit_message>
vendor login and forget password validations
</commit_message>
<xml_diff>
--- a/excel/TestData.xlsx
+++ b/excel/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6470" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="6470"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>uday@malaysiaairports.com.my</t>
+  </si>
+  <si>
+    <t>palepu</t>
   </si>
   <si>
     <t>password</t>
@@ -1184,13 +1187,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15" customHeight="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="42.1363636363636" customWidth="1"/>
@@ -1198,7 +1201,7 @@
     <col min="4" max="26" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" spans="1:3">
+    <row r="1" ht="14.25" customHeight="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,35 +1211,38 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1"/>
@@ -2254,7 +2260,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>